<commit_message>
Added bag. Added E/R model. Chanmged CSV files for Disc ownership
</commit_message>
<xml_diff>
--- a/excel documents/disc.xlsx
+++ b/excel documents/disc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\github\1dv503\database_assignment3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\github\1dv503\database_assignment3\excel documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01BCAB5-EB7B-4482-B0C4-5BCB01926C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD4337F-24C9-4605-B5FD-1B5F9E188898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14580" yWindow="4035" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4605" yWindow="6810" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>weigth</t>
-  </si>
-  <si>
     <t>speed</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>Pain</t>
+  </si>
+  <si>
+    <t>max_weigth</t>
   </si>
 </sst>
 </file>
@@ -417,7 +417,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,36 +433,36 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>178</v>
@@ -480,7 +480,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2">
         <v>60</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>179</v>
@@ -512,7 +512,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3">
         <v>45</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>181</v>
@@ -544,7 +544,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4">
         <v>50</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>176</v>
@@ -576,7 +576,7 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5">
         <v>60</v>
@@ -590,7 +590,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>175</v>
@@ -608,7 +608,7 @@
         <v>3.5</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H6">
         <v>70</v>
@@ -622,7 +622,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>175</v>
@@ -640,7 +640,7 @@
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7">
         <v>75</v>
@@ -654,7 +654,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>176</v>
@@ -672,7 +672,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8">
         <v>40</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>175</v>
@@ -704,7 +704,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H9">
         <v>40</v>
@@ -718,7 +718,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <v>176</v>
@@ -736,7 +736,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H10">
         <v>40</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>180</v>
@@ -768,7 +768,7 @@
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11">
         <v>55</v>

</xml_diff>